<commit_message>
Attempt at markdown pipeline
</commit_message>
<xml_diff>
--- a/data_sources.xlsx
+++ b/data_sources.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Keith/Dev/research/johns-hopkins/dredze/mental-health-datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5868442F-3CDC-A24F-AE8F-223CA6FC2F1B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD87C4E8-6E49-7343-B9EF-E9214E9106AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="280" yWindow="460" windowWidth="26740" windowHeight="14420" xr2:uid="{12AC74CC-1E53-1243-8351-D86244D05D7E}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="267">
   <si>
     <t>Paper</t>
   </si>
@@ -580,9 +580,6 @@
   </si>
   <si>
     <t>Pisani, Kanuri, Filbin, Gallo, Gould, Lehmann, Levine, Marcotte, Pascal, Rousseau, Turner, Yen, Ranney</t>
-  </si>
-  <si>
-    <t>N/A</t>
   </si>
   <si>
     <t>https://www.jmir.org/2019/1/e11507/</t>
@@ -1214,8 +1211,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50E2654E-11BF-434E-B104-18FED2D9E566}">
   <dimension ref="A1:K44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G7" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="30.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2066,10 +2063,10 @@
         <v>160</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>178</v>
+        <v>52</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>178</v>
+        <v>52</v>
       </c>
       <c r="G30" s="1" t="s">
         <v>162</v>
@@ -2078,125 +2075,125 @@
         <v>163</v>
       </c>
       <c r="K30" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="85" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="B31" s="1" t="s">
         <v>180</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>181</v>
       </c>
       <c r="C31" s="1">
         <v>2014</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>65</v>
       </c>
       <c r="F31" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="G31" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="G31" s="1" t="s">
+      <c r="K31" s="1" t="s">
         <v>184</v>
-      </c>
-      <c r="K31" s="1" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="32" spans="1:11" ht="51" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="B32" s="1" t="s">
         <v>186</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>187</v>
       </c>
       <c r="C32" s="1">
         <v>2016</v>
       </c>
       <c r="D32" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="E32" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="E32" s="1" t="s">
+      <c r="F32" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="F32" s="1" t="s">
+      <c r="G32" s="1" t="s">
         <v>190</v>
-      </c>
-      <c r="G32" s="1" t="s">
-        <v>191</v>
       </c>
       <c r="H32" s="1" t="s">
         <v>17</v>
       </c>
       <c r="K32" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="33" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B33" s="1" t="s">
         <v>193</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>194</v>
       </c>
       <c r="C33" s="1">
         <v>2018</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>132</v>
       </c>
       <c r="F33" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="G33" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="G33" s="1" t="s">
+      <c r="I33" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="I33" s="1" t="s">
+      <c r="K33" s="1" t="s">
         <v>198</v>
-      </c>
-      <c r="K33" s="1" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="34" spans="1:11" ht="51" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="B34" s="1" t="s">
         <v>200</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>201</v>
       </c>
       <c r="C34" s="1">
         <v>2019</v>
       </c>
       <c r="D34" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="E34" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="E34" s="1" t="s">
+      <c r="F34" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="F34" s="1" t="s">
+      <c r="G34" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="G34" s="1" t="s">
+      <c r="K34" s="1" t="s">
         <v>205</v>
-      </c>
-      <c r="K34" s="1" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="35" spans="1:11" ht="289" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="B35" s="1" t="s">
         <v>207</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>208</v>
       </c>
       <c r="C35" s="1">
         <v>2018</v>
@@ -2208,53 +2205,53 @@
         <v>132</v>
       </c>
       <c r="F35" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="G35" s="1" t="s">
         <v>209</v>
-      </c>
-      <c r="G35" s="1" t="s">
-        <v>210</v>
       </c>
       <c r="H35" s="1" t="s">
         <v>17</v>
       </c>
       <c r="K35" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="36" spans="1:11" ht="51" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="B36" s="1" t="s">
         <v>212</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>213</v>
       </c>
       <c r="C36" s="1">
         <v>2018</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>132</v>
       </c>
       <c r="F36" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="G36" s="1" t="s">
         <v>215</v>
-      </c>
-      <c r="G36" s="1" t="s">
-        <v>216</v>
       </c>
       <c r="H36" s="1" t="s">
         <v>174</v>
       </c>
       <c r="K36" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="37" spans="1:11" ht="68" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="B37" s="1" t="s">
         <v>218</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>219</v>
       </c>
       <c r="C37" s="1">
         <v>2017</v>
@@ -2266,27 +2263,27 @@
         <v>65</v>
       </c>
       <c r="F37" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="G37" s="1" t="s">
         <v>220</v>
-      </c>
-      <c r="G37" s="1" t="s">
-        <v>221</v>
       </c>
       <c r="H37" s="1" t="s">
         <v>17</v>
       </c>
       <c r="J37" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="K37" s="1" t="s">
         <v>222</v>
-      </c>
-      <c r="K37" s="1" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="38" spans="1:11" ht="68" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="B38" s="1" t="s">
         <v>224</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>225</v>
       </c>
       <c r="C38" s="1">
         <v>2017</v>
@@ -2295,24 +2292,24 @@
         <v>13</v>
       </c>
       <c r="E38" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="F38" s="1" t="s">
         <v>226</v>
-      </c>
-      <c r="F38" s="1" t="s">
-        <v>227</v>
       </c>
       <c r="G38" s="1" t="s">
         <v>47</v>
       </c>
       <c r="K38" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="39" spans="1:11" ht="102" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="B39" s="1" t="s">
         <v>229</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>230</v>
       </c>
       <c r="C39" s="1">
         <v>2019</v>
@@ -2324,24 +2321,24 @@
         <v>132</v>
       </c>
       <c r="F39" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="G39" s="1" t="s">
         <v>231</v>
-      </c>
-      <c r="G39" s="1" t="s">
-        <v>232</v>
       </c>
       <c r="H39" s="1" t="s">
         <v>17</v>
       </c>
       <c r="K39" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="40" spans="1:11" ht="136" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="B40" s="1" t="s">
         <v>234</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>235</v>
       </c>
       <c r="C40" s="1">
         <v>2016</v>
@@ -2350,27 +2347,27 @@
         <v>13</v>
       </c>
       <c r="E40" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="F40" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="F40" s="1" t="s">
+      <c r="G40" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="G40" s="1" t="s">
+      <c r="H40" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="H40" s="1" t="s">
+      <c r="K40" s="1" t="s">
         <v>239</v>
-      </c>
-      <c r="K40" s="1" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="41" spans="1:11" ht="68" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="B41" s="1" t="s">
         <v>241</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>242</v>
       </c>
       <c r="C41" s="1">
         <v>2019</v>
@@ -2379,27 +2376,27 @@
         <v>125</v>
       </c>
       <c r="E41" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="F41" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="F41" s="1" t="s">
+      <c r="G41" s="1" t="s">
         <v>244</v>
-      </c>
-      <c r="G41" s="1" t="s">
-        <v>245</v>
       </c>
       <c r="H41" s="1" t="s">
         <v>60</v>
       </c>
       <c r="K41" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="42" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="B42" s="1" t="s">
         <v>247</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>248</v>
       </c>
       <c r="C42" s="1">
         <v>2015</v>
@@ -2408,27 +2405,27 @@
         <v>13</v>
       </c>
       <c r="E42" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="F42" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="F42" s="1" t="s">
+      <c r="G42" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="G42" s="1" t="s">
+      <c r="J42" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="J42" s="1" t="s">
+      <c r="K42" s="1" t="s">
         <v>252</v>
-      </c>
-      <c r="K42" s="1" t="s">
-        <v>253</v>
       </c>
     </row>
     <row r="43" spans="1:11" ht="153" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="B43" s="1" t="s">
         <v>254</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>255</v>
       </c>
       <c r="C43" s="1">
         <v>2018</v>
@@ -2437,30 +2434,30 @@
         <v>106</v>
       </c>
       <c r="E43" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="F43" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="F43" s="1" t="s">
+      <c r="G43" s="1" t="s">
         <v>257</v>
-      </c>
-      <c r="G43" s="1" t="s">
-        <v>258</v>
       </c>
       <c r="H43" s="1" t="s">
         <v>17</v>
       </c>
       <c r="J43" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="K43" s="1" t="s">
         <v>259</v>
-      </c>
-      <c r="K43" s="1" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="44" spans="1:11" ht="51" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="B44" s="1" t="s">
         <v>261</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>262</v>
       </c>
       <c r="C44" s="1">
         <v>2018</v>
@@ -2469,22 +2466,22 @@
         <v>106</v>
       </c>
       <c r="E44" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="F44" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="F44" s="1" t="s">
+      <c r="G44" s="1" t="s">
         <v>264</v>
-      </c>
-      <c r="G44" s="1" t="s">
-        <v>265</v>
       </c>
       <c r="H44" s="1" t="s">
         <v>17</v>
       </c>
       <c r="J44" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="K44" s="1" t="s">
         <v>266</v>
-      </c>
-      <c r="K44" s="1" t="s">
-        <v>267</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated dataset list and README
</commit_message>
<xml_diff>
--- a/data_sources.xlsx
+++ b/data_sources.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Keith/Dev/research/johns-hopkins/dredze/mental-health-datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3F812FD-A310-6A4E-B96B-38E94745EEDC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{321FFF2B-F5A5-DB4B-BC46-F737525E614E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="280" yWindow="460" windowWidth="26740" windowHeight="14420" xr2:uid="{12AC74CC-1E53-1243-8351-D86244D05D7E}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="13660" windowHeight="14900" xr2:uid="{12AC74CC-1E53-1243-8351-D86244D05D7E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="392">
   <si>
     <t>Paper</t>
   </si>
@@ -855,6 +855,387 @@
   </si>
   <si>
     <t>Sing, Nair, Zirikly, Friedenberg, Daumé III, Resnik</t>
+  </si>
+  <si>
+    <t>Towards Developing an Annotation Scheme for Depressive Disorder Symptoms: A Preliminary Study using Twitter Data</t>
+  </si>
+  <si>
+    <t>Mowery, Bryan, Conway</t>
+  </si>
+  <si>
+    <t>Major Depressive Disorder</t>
+  </si>
+  <si>
+    <t>129 Tweets</t>
+  </si>
+  <si>
+    <t>Manual Annotation, hierarchical schema. Data queried from API using keywords.</t>
+  </si>
+  <si>
+    <t>Pilot Study</t>
+  </si>
+  <si>
+    <t>https://www.aclweb.org/anthology/W15-1211/</t>
+  </si>
+  <si>
+    <t>Automatically Generating Pschiatric Case Note From Digital Transcripts of Doctor-Patient Conversations</t>
+  </si>
+  <si>
+    <t>Kazi, Kahanda</t>
+  </si>
+  <si>
+    <t>EHR Categories: Client Details, Chief Complaint, Family History, Social History, Medical History, Other</t>
+  </si>
+  <si>
+    <t>18 Doctor-patient Transcripts (13 synthetic)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://search.alexanderstreet.com/health- sciences/counseling-therapy </t>
+  </si>
+  <si>
+    <t>https://www.aclweb.org/anthology/W19-1918/</t>
+  </si>
+  <si>
+    <t>Detecting Changes in Suicide Content Manifested in Social Media Following Celebrity Suicides</t>
+  </si>
+  <si>
+    <t>Kumar, Dredze, Coppersmith, De Choudury</t>
+  </si>
+  <si>
+    <t>Reddit, Wikipedia</t>
+  </si>
+  <si>
+    <t>Participation in r/SuicideWatch</t>
+  </si>
+  <si>
+    <t>https://www.ncbi.nlm.nih.gov/pmc/articles/PMC5507358/</t>
+  </si>
+  <si>
+    <t>Using Linguistic Features to Estimate Suicide Probability of Chinese Microblog Users</t>
+  </si>
+  <si>
+    <t>Zhang, Huang, Liu, Chen, Zhu</t>
+  </si>
+  <si>
+    <t>Sina Weibo</t>
+  </si>
+  <si>
+    <t>Survey (Suicide Probability Scale)</t>
+  </si>
+  <si>
+    <t>https://link.springer.com/chapter/10.1007/978-3-319-15554-8_45</t>
+  </si>
+  <si>
+    <t>Identifying Chinese Microblog Users with High Suicide Probability Using Internet-Based Profile and Linguistic Features: Classification Model</t>
+  </si>
+  <si>
+    <t>Guan, Hao, Cheng, Yip, Zhu</t>
+  </si>
+  <si>
+    <t>https://www.ncbi.nlm.nih.gov/pubmed/26543921</t>
+  </si>
+  <si>
+    <t>Detecting Suicidal Ideation in Chinese Microblogs with Psychological Lexicons</t>
+  </si>
+  <si>
+    <t>Huang, Zhang, Liu, Chiu, Li, Zhu</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/abs/1411.0778</t>
+  </si>
+  <si>
+    <t>Distinguishing Clinical Sentiment: The Importance of Domain Adaptation in Psychiatric Patient Health Records</t>
+  </si>
+  <si>
+    <t>Holderness, Cawkwell, Bolton, Pustejovsky, Hall</t>
+  </si>
+  <si>
+    <t>EHR</t>
+  </si>
+  <si>
+    <t>EHR Categories: Appearance, Mood, Interpersonal, Substance Use, Occupation, Thought Content, Thought Process</t>
+  </si>
+  <si>
+    <t>Manual Annotation (see Holderness et al., 2018)</t>
+  </si>
+  <si>
+    <t>4,500 Sentences</t>
+  </si>
+  <si>
+    <t>https://www.aclweb.org/anthology/W19-1915/</t>
+  </si>
+  <si>
+    <t>The Language of Social Support in Social edia and its Effect on Suicidal Ideation Risk</t>
+  </si>
+  <si>
+    <t>De Choudury, Kiciman</t>
+  </si>
+  <si>
+    <t>Subreddit Participation; classes distinguished based on timeperiod of posting and movement between r/SuicideWatch and other mental-health subreddits</t>
+  </si>
+  <si>
+    <t>909 individuals</t>
+  </si>
+  <si>
+    <t>1,053 individuals (6,754 posts)</t>
+  </si>
+  <si>
+    <t>1,038 individuals (Up to 2,000 messages)</t>
+  </si>
+  <si>
+    <t>66,059 posts from 19,159 individuals</t>
+  </si>
+  <si>
+    <t>440 individuals MH to SW (62,024 comments of support from 32,362 unique users);
+440 individuals MH (41,894 comments of support from 21,358 unique users)</t>
+  </si>
+  <si>
+    <t>https://www.microsoft.com/en-us/research/publication/language-social-support-social-media-effect-suicidal-ideation-risk/</t>
+  </si>
+  <si>
+    <t>Mental Health Surveillance over Social Media with Digital Cohorts</t>
+  </si>
+  <si>
+    <t>Amir, Dredze, Ayers</t>
+  </si>
+  <si>
+    <t>https://www.aclweb.org/anthology/W19-3013/</t>
+  </si>
+  <si>
+    <t>Natural language processing to extract symptoms of severe mental illness from clinical text: the Clinical Record Interactive Search Comprehensive Data Extraction (CRIS-CODE) project</t>
+  </si>
+  <si>
+    <t>Jackson, Patel, Jayatilleke, Kolliakou, Ball, Gorrell, Roberts, Dobson, Stewart</t>
+  </si>
+  <si>
+    <t>Psychiatric concepts</t>
+  </si>
+  <si>
+    <t>Regular expressions; manual verification for 15 of the concepts; 50 concepts total</t>
+  </si>
+  <si>
+    <t>37,211 instances (training)
+2,950 instances (testing)</t>
+  </si>
+  <si>
+    <t>https://bmjopen.bmj.com/content/7/1/e012012</t>
+  </si>
+  <si>
+    <t>Feature Attention Network: Interpretable Depression Detection from Social Media</t>
+  </si>
+  <si>
+    <t>Song, You, Chunk, Park</t>
+  </si>
+  <si>
+    <t>https://www.aclweb.org/anthology/Y18-1070/</t>
+  </si>
+  <si>
+    <t>Natural Language Processing for Mental Health: Large Scale Discourse Analysis of Counseling Conversations</t>
+  </si>
+  <si>
+    <t>Althoff, Clark, Leskovec</t>
+  </si>
+  <si>
+    <t>Counseling Outcome</t>
+  </si>
+  <si>
+    <t>Survey (interactive text-messaging sessions) regarding success of session</t>
+  </si>
+  <si>
+    <t>408 counselors; 3.2 million messages; 80,885 conversations</t>
+  </si>
+  <si>
+    <t>http://snap.stanford.edu/counseling/</t>
+  </si>
+  <si>
+    <t>http://timalthoff.com/docs/althoff-2016-mental_health.pdf</t>
+  </si>
+  <si>
+    <t>The Role of Features and Context on Suicide Ideation Detection</t>
+  </si>
+  <si>
+    <t>Wang, Wan, Paris</t>
+  </si>
+  <si>
+    <t>https://www.aclweb.org/anthology/U16-1010/</t>
+  </si>
+  <si>
+    <t>Davcheva, Adam, Benlian</t>
+  </si>
+  <si>
+    <t>3 Online mental-health forums</t>
+  </si>
+  <si>
+    <t>Sentiment</t>
+  </si>
+  <si>
+    <t>Forum participation (Depression, Bipolar Disorder, Anxiety, Panic Attacks, ADHD, Borderline Personality Disorder, OCD, PTSD)</t>
+  </si>
+  <si>
+    <t>49,113 threads; 500,754 posts; 75,000 individuals</t>
+  </si>
+  <si>
+    <t>2,000 posts (14% high, 56% possibly, 29% safe)</t>
+  </si>
+  <si>
+    <t>https://aisel.aisnet.org/cgi/viewcontent.cgi?article=1269&amp;context=wi2019</t>
+  </si>
+  <si>
+    <t>User Dynamics in Mental Health Forums -- A Sentiment Analysis Perspective</t>
+  </si>
+  <si>
+    <t>Using Automated Metaphor Identification to Aid in Detection and Prediction of First-Episode Schizophrenia</t>
+  </si>
+  <si>
+    <t>Guitiérrez, Corlett, Corcoran, Cecchi</t>
+  </si>
+  <si>
+    <t>Patient Interviews (First-episode Schizophrenia and Prodomal Syndromes)</t>
+  </si>
+  <si>
+    <t>First-episode: 17 patients and 15 healthy controls
+Prodomal Psychosis: 34 individuals at clinical high risk for psychosis</t>
+  </si>
+  <si>
+    <t>https://www.aclweb.org/anthology/D17-1316/</t>
+  </si>
+  <si>
+    <t>Automated analysis of free speech predicts psychosis onset in high-risk youth</t>
+  </si>
+  <si>
+    <t>Bedi, Carrillo, Cecchi, Fernández Slezak, Sigman, Mota, Ribeiro, Javitt, Copelli, Corcoran</t>
+  </si>
+  <si>
+    <t>Patient Interviews</t>
+  </si>
+  <si>
+    <t>Schizophrenhia, Psychosis</t>
+  </si>
+  <si>
+    <t>Psychosis</t>
+  </si>
+  <si>
+    <t>Schizophrenia, Psychosis Diagnoses</t>
+  </si>
+  <si>
+    <t>Psychosis Diagnoses</t>
+  </si>
+  <si>
+    <t>34 individuals at clinical high risk for psychosis</t>
+  </si>
+  <si>
+    <t>https://www.nature.com/articles/npjschz201530</t>
+  </si>
+  <si>
+    <t>Adapting Deep Learning Methods for Mental Health Prediction on Social Media</t>
+  </si>
+  <si>
+    <t>Sekulic, Strube</t>
+  </si>
+  <si>
+    <t>https://www.aclweb.org/anthology/D19-5542/</t>
+  </si>
+  <si>
+    <t>Multi-Task, Multi-Channel, Multi-Input Learning for Mental Illness Detection using Social Media Text</t>
+  </si>
+  <si>
+    <t>Kirinde Gamaarachichige, Inkpen</t>
+  </si>
+  <si>
+    <t>https://www.aclweb.org/anthology/D19-6208/</t>
+  </si>
+  <si>
+    <t>Assessing the Efficacy of Clinical Sentiment Analysis and Topic Extraction in Psychiatric Readmission Risk Prediction</t>
+  </si>
+  <si>
+    <t>Alvarez-Mellado, Holderness, Miller, Dhang, Cawkwell, Bolton, Putesjovsky, Hall</t>
+  </si>
+  <si>
+    <t>Psychiatric Readmission</t>
+  </si>
+  <si>
+    <t>Medical history</t>
+  </si>
+  <si>
+    <t>2,346 clinical notes for 183 patients</t>
+  </si>
+  <si>
+    <t>https://www.aclweb.org/anthology/D19-6211/</t>
+  </si>
+  <si>
+    <t>Dreaddit: A Reddit Dataset for Stress Analysis in Social Media</t>
+  </si>
+  <si>
+    <t>Turcan, McKeown</t>
+  </si>
+  <si>
+    <t>Stress</t>
+  </si>
+  <si>
+    <t>Manual annotation via Mechanical Turk (Stress, Not Stress, Can't Tell)</t>
+  </si>
+  <si>
+    <t>3,554 labeled data points for 2,929 posts</t>
+  </si>
+  <si>
+    <t>http://www.cs.columbia.edu/~eturcan/data/dreaddit.zip</t>
+  </si>
+  <si>
+    <t>https://www.aclweb.org/anthology/D19-6213/</t>
+  </si>
+  <si>
+    <t>Dilated LSTM with attention for Classification of Suicide Notes</t>
+  </si>
+  <si>
+    <t>Schoene, Lacy, Turner, Dethlefs</t>
+  </si>
+  <si>
+    <t>Death Row Last Statements, The Kernel/Tumblr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Last Row Death Row (Texas Department of Criminal Justices); </t>
+  </si>
+  <si>
+    <t>Suicide, Imminent Death, Depression, Lonliness</t>
+  </si>
+  <si>
+    <t>Last Statements: 431 notes
+Suicide Notes: 161 notes
+Depression Notes: 142 notes</t>
+  </si>
+  <si>
+    <t>https://www.aclweb.org/anthology/D19-6217/</t>
+  </si>
+  <si>
+    <t>Latent Suicide Risk Detection on Microblog via Suicide-Oriented Word Embeddings and Layered Attention</t>
+  </si>
+  <si>
+    <t>Cao, Zhang, Feng, Wei, Wang, Li, He</t>
+  </si>
+  <si>
+    <t>Commenting in "Tree Hole" (a page on Sina Weibo from an individual who died by suicide)</t>
+  </si>
+  <si>
+    <t>7,329 individuals</t>
+  </si>
+  <si>
+    <t>https://www.aclweb.org/anthology/D19-1181/</t>
+  </si>
+  <si>
+    <t>Gender and Cross-Cultural Differences in Social Media Disclosures of Mental Illness</t>
+  </si>
+  <si>
+    <t>De Choudury, Sharma, Logar, Eekhout, Cluasen Nielsen</t>
+  </si>
+  <si>
+    <t>Regular expressions</t>
+  </si>
+  <si>
+    <t>Candidate disclosures: 51,038,914 posts from 470,337 individuals
+Control: 66,214,850 posts from 480,685 individuals</t>
+  </si>
+  <si>
+    <t>https://dl.acm.org/citation.cfm?id=2998220</t>
   </si>
 </sst>
 </file>
@@ -890,9 +1271,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1209,10 +1594,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50E2654E-11BF-434E-B104-18FED2D9E566}">
-  <dimension ref="A1:K44"/>
+  <dimension ref="A1:K67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView tabSelected="1" topLeftCell="E61" zoomScale="125" workbookViewId="0">
+      <selection activeCell="K68" sqref="K68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="30.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2484,6 +2869,670 @@
         <v>265</v>
       </c>
     </row>
+    <row r="45" spans="1:11" ht="68" x14ac:dyDescent="0.2">
+      <c r="A45" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="C45" s="1">
+        <v>2015</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="H45" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="I45" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="K45" s="1" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" ht="68" x14ac:dyDescent="0.2">
+      <c r="A46" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="C46" s="1">
+        <v>2019</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="J46" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="K46" s="1" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+      <c r="A47" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="C47" s="1">
+        <v>2015</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="H47" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="K47" s="1" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+      <c r="A48" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="C48" s="1">
+        <v>2014</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="I48" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="K48" s="1" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" ht="85" x14ac:dyDescent="0.2">
+      <c r="A49" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="C49" s="1">
+        <v>2015</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="I49" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="K49" s="1" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+      <c r="A50" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="C50" s="1">
+        <v>2014</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="I50" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="K50" s="1" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" ht="68" x14ac:dyDescent="0.2">
+      <c r="A51" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="C51" s="1">
+        <v>2019</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="K51" s="2" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" ht="102" x14ac:dyDescent="0.2">
+      <c r="A52" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="C52" s="1">
+        <v>2017</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="G52" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="H52" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="K52" s="1" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" ht="68" x14ac:dyDescent="0.2">
+      <c r="A53" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="C53" s="1">
+        <v>2019</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H53" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K53" s="1" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" ht="102" x14ac:dyDescent="0.2">
+      <c r="A54" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="C54" s="1">
+        <v>2017</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="G54" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="K54" s="1" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" ht="68" x14ac:dyDescent="0.2">
+      <c r="A55" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="C55" s="1">
+        <v>2018</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="G55" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="H55" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J55" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="K55" s="1" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" ht="68" x14ac:dyDescent="0.2">
+      <c r="A56" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="C56" s="1">
+        <v>2016</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="G56" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="H56" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="J56" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="K56" s="1" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+      <c r="A57" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="C57" s="1">
+        <v>2019</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="G57" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="H57" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="K57" s="1" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" ht="68" x14ac:dyDescent="0.2">
+      <c r="A58" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="C58" s="1">
+        <v>2019</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="G58" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="K58" s="1" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" ht="68" x14ac:dyDescent="0.2">
+      <c r="A59" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C59" s="1">
+        <v>2017</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="G59" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="H59" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K59" s="1" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+      <c r="A60" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="C60" s="1">
+        <v>2015</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="G60" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="H60" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K60" s="1" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" ht="68" x14ac:dyDescent="0.2">
+      <c r="A61" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="C61" s="1">
+        <v>2019</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="G61" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="H61" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J61" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="K61" s="1" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" ht="68" x14ac:dyDescent="0.2">
+      <c r="A62" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="C62" s="1">
+        <v>2019</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G62" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H62" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K62" s="1" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" ht="68" x14ac:dyDescent="0.2">
+      <c r="A63" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="C63" s="1">
+        <v>2019</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="G63" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="K63" s="1" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+      <c r="A64" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="C64" s="1">
+        <v>2019</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="G64" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="H64" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="J64" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="K64" s="1" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+      <c r="A65" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="C65" s="1">
+        <v>2019</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="G65" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="K65" s="1" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" ht="68" x14ac:dyDescent="0.2">
+      <c r="A66" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="C66" s="1">
+        <v>2019</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="F66" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="G66" s="3" t="s">
+        <v>385</v>
+      </c>
+      <c r="I66" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="K66" s="1" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" ht="68" x14ac:dyDescent="0.2">
+      <c r="A67" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="C67" s="1">
+        <v>2017</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="F67" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="G67" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="K67" s="1" t="s">
+        <v>391</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Standardized format of data sources (less specific)
</commit_message>
<xml_diff>
--- a/data_sources.xlsx
+++ b/data_sources.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Keith/Dev/research/johns-hopkins/dredze/mental-health-datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA56CEFF-63CE-A346-AFA8-184434F880F8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{878135BB-13DE-B04D-B8FF-564CDD84247C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13660" yWindow="460" windowWidth="13660" windowHeight="14900" xr2:uid="{12AC74CC-1E53-1243-8351-D86244D05D7E}"/>
   </bookViews>
@@ -1687,8 +1687,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50E2654E-11BF-434E-B104-18FED2D9E566}">
   <dimension ref="A1:K72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G40" zoomScale="86" workbookViewId="0">
-      <selection activeCell="I43" sqref="I43"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="86" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="30.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>